<commit_message>
Aktualizace objednávky na GVD 14.6.
</commit_message>
<xml_diff>
--- a/2025/MAVIS_objednavka_Boh_GVD25.xlsx
+++ b/2025/MAVIS_objednavka_Boh_GVD25.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OIS\CD\Data\2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{083009A6-8E14-41E3-9CA6-B03AA0FEE4B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{767D6B26-82D8-48E3-8FE0-F03C616AEA8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="1080" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regio_razeni" sheetId="1" r:id="rId1"/>
@@ -118,9 +118,6 @@
     <t>vše nová (kromě 471)</t>
   </si>
   <si>
-    <t>1600 - 1633, 1635, 1650, 1651, 2040 - 2047, 2800 - 2803, 2805, 2807, 2809, 2851, 2860 - 2862, 2864 - 2872, 2874 - 2879, 2887, 2889, 2892, 2896, 2898, 2900, 2915, 2921, 2923 - 2940, 2942 - 2957, 2990 - 2997, 3000, 3002, 3010 - 3032, 3034, 3040 - 3045, 3058, 3066, 3067, 3073 - 3075, 3077, 3081 - 3086, 3088 - 3141, 3143, 3144, 3146 - 3157, 3159 - 3161, 3170, 3171, 3180 - 3182, 3190, 3192, 3194, 3196, 3197, 3300 - 3325, 3348, 3350 - 3357, 3359 - 3366, 3368 - 3383, 3385, 3387, 3390, 3393 - 3396, 3398 - 3438, 3440, 3441, 3486, 3488, 3495, 3497, 3900 - 3939, 3941, 3943 - 3954, 3956, 3958, 3960 - 3963, 3965, 3966, 3980 - 3984, 3986, 3990, 4232, 4235, 4238, 4240 - 4242, 4244 - 4247, 12800 - 12823, 12826, 12827, 12830, 12831, 12834, 12835, 12838, 12839, 12842 - 12853, 12860 - 12863, 12900 - 12939, 13100, 13104, 13105, 13107 - 13119, 13122 - 13141, 13144, 13171, 13173 - 13191, 13193 - 13196, 13198, 13199, 13201 - 13211, 13213 - 13227, 13229, 13300 - 13316, 13320 - 13328, 13330, 13332, 13334, 13340 - 13346, 13351, 13354 - 13386, 13390 - 13395, 13901 - 13918, 13925, 13926, 14200 - 14256, 14261, 14262, 14264 - 14266, 14272 - 14275, 23100 - 23109, 23140, 23158, 23166, 23167, 23174, 23175, 23182, 23183, 23189 - 23191, 23300 - 23333, 23352 - 23375, 28900 - 28904, 28906, 28907, 28909, 28911, 28912, 28915, 28917, 28918, 28920 - 28922, 28930, 28931, 28933 - 28935, 28937, 28940 - 28942, 28944, 28948, 28949</t>
-  </si>
-  <si>
     <t>vše nová (kromě 471 - ty stále nejsou)</t>
   </si>
   <si>
@@ -133,9 +130,6 @@
     <t>dálková</t>
   </si>
   <si>
-    <t>101, 104, 110 - 117, 123, 124, 128 - 131, 140 - 145, 212, 213, 223, 240, 241, 271, 273, 274, 276, 341 - 343, 402 - 405, 518, 520, 546, 547, 549, 579, 858, 876, 879 - 897, 29143, 29341 - 29343, 29894, 50175, 55174</t>
-  </si>
-  <si>
     <t>Olomouc hl. n.</t>
   </si>
   <si>
@@ -143,6 +137,12 @@
   </si>
   <si>
     <t>Ostrava hl. n.</t>
+  </si>
+  <si>
+    <t>1600, 1602, 1605 - 1614, 1616 - 1621, 1623 - 1634, 1650, 1651, 2031 - 2033, 2035, 2039 - 2045, 2800 - 2803, 2805, 2807, 2809, 2851, 2860 - 2862, 2864, 2865, 2868 - 2872, 2874 - 2879, 2885, 2886, 2888, 2892, 2900, 2915, 2921, 2923 - 2940, 2942 - 2957, 2990 - 2992, 2994 - 2997, 2999, 3000, 3002, 3010 - 3032, 3034, 3040 - 3045, 3050, 3054, 3058, 3062, 3063, 3066, 3067, 3070, 3071, 3073 - 3075, 3077 - 3079, 3081 - 3141, 3143, 3144, 3146 - 3157, 3159 - 3161, 3170 - 3175, 3180 - 3182, 3190, 3192, 3194, 3196, 3197, 3300 - 3325, 3348, 3350 - 3377, 3379 - 3383, 3385, 3388, 3390, 3398 - 3438, 3440, 3441, 3900 - 3939, 3941, 3943 - 3954, 3956, 3958, 3960 - 3963, 3965, 3966, 3980 - 3984, 3986, 3990, 4232, 4235, 4238, 4240 - 4242, 4244 - 4247, 4275, 4276, 12800 - 12823, 12826, 12827, 12830, 12831, 12834, 12835, 12838, 12839, 12842 - 12853, 12855, 12860 - 12863, 12890, 12900 - 12939, 12950 - 12955, 12960, 12961, 13100, 13104, 13105, 13107 - 13119, 13122 - 13141, 13144, 13171, 13173 - 13191, 13193 - 13199, 13201 - 13211, 13213 - 13227, 13229, 13300 - 13316, 13320 - 13328, 13330, 13334, 13340 - 13346, 13351, 13354 - 13386, 13390 - 13395, 13901 - 13918, 13925, 13926, 14200 - 14256, 14261, 14262, 14264 - 14266, 14272 - 14275, 23100 - 23109, 23140, 23142, 23144, 23150, 23154, 23158, 23162, 23163, 23166, 23167, 23170, 23171, 23174, 23175, 23178, 23179, 23182, 23183, 23187, 23189 - 23195, 23197, 23199, 23300 - 23333, 23352 - 23375, 28900 - 28904, 28906 - 28913, 28915, 28917, 28918, 28920 - 28922, 28930, 28931, 28933 - 28935, 28937 - 28942, 28944, 28948, 28949, 103399</t>
+  </si>
+  <si>
+    <t>101, 104, 110 - 117, 120, 123, 128, 130, 131, 140 - 145, 212, 213, 221, 223, 240, 241, 271, 273, 274, 276, 341 - 343, 402 - 405, 512, 515, 518, 520, 546, 547, 549, 579, 858, 876, 879 - 897, 29143, 29341 - 29343, 29894, 50175, 55174</t>
   </si>
 </sst>
 </file>
@@ -195,30 +195,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -527,7 +523,7 @@
   <dimension ref="A1:C49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -538,265 +534,231 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="6"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="6"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="6"/>
+      <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B6" s="3"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="2"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="2"/>
+      <c r="B9" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="6"/>
+      <c r="B10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="5"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="2">
         <v>1440</v>
       </c>
-      <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="3">
-        <v>2</v>
-      </c>
-      <c r="C12" s="2"/>
+      <c r="B12" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" s="2"/>
+      <c r="B13" s="4" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+      <c r="A14" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="2"/>
+      <c r="B14" s="4" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" s="2"/>
+      <c r="B15" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16" s="2"/>
+      <c r="B16" s="4" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+      <c r="A17" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C17" s="2"/>
+      <c r="B17" s="3" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+      <c r="A18" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C18" s="2"/>
+      <c r="B18" s="3" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
+      <c r="A19" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C19" s="2"/>
+      <c r="B19" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="2"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="2"/>
+      <c r="B20" s="3"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="6" t="s">
+      <c r="B21" s="3"/>
+      <c r="C21" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="153" x14ac:dyDescent="0.2">
-      <c r="A22" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B22" s="4"/>
+    <row r="22" spans="1:3" ht="178.5" x14ac:dyDescent="0.2">
+      <c r="A22" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="3"/>
       <c r="C22" s="1"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="2"/>
-      <c r="B34" s="4"/>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B34" s="3"/>
       <c r="C34" s="1"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="2"/>
-      <c r="B35" s="4"/>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B35" s="3"/>
       <c r="C35" s="1"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="2"/>
-      <c r="B36" s="4"/>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B36" s="3"/>
       <c r="C36" s="1"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="2"/>
-      <c r="B37" s="4"/>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B37" s="3"/>
       <c r="C37" s="1"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="2"/>
-      <c r="B38" s="4"/>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B38" s="3"/>
       <c r="C38" s="1"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="2"/>
-      <c r="B39" s="4"/>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B39" s="3"/>
       <c r="C39" s="1"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="2"/>
-      <c r="B40" s="4"/>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B40" s="3"/>
       <c r="C40" s="1"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="7"/>
-      <c r="B41" s="4"/>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B41" s="3"/>
       <c r="C41" s="1"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="7"/>
-      <c r="B42" s="4"/>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B42" s="3"/>
       <c r="C42" s="1"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="7"/>
-      <c r="B43" s="4"/>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B43" s="3"/>
       <c r="C43" s="1"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="7"/>
-      <c r="B44" s="4"/>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B44" s="3"/>
       <c r="C44" s="1"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="7"/>
-      <c r="B45" s="4"/>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B45" s="3"/>
       <c r="C45" s="1"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="7"/>
-      <c r="B46" s="4"/>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B46" s="3"/>
       <c r="C46" s="1"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="7"/>
-      <c r="B47" s="4"/>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B47" s="3"/>
       <c r="C47" s="1"/>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" s="7"/>
-      <c r="B48" s="4"/>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B48" s="3"/>
       <c r="C48" s="1"/>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" s="7"/>
-      <c r="B49" s="4"/>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B49" s="3"/>
       <c r="C49" s="1"/>
     </row>
   </sheetData>
@@ -827,183 +789,165 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="8"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="8"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="8"/>
+      <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="2"/>
+      <c r="B6" s="3"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="A7" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="A8" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="2"/>
+      <c r="B8" s="4"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="2"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="8"/>
+      <c r="C10" s="5"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="2">
         <v>0</v>
       </c>
-      <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="3">
-        <v>2</v>
-      </c>
-      <c r="C12" s="2"/>
+      <c r="B12" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" s="2"/>
+      <c r="B13" s="4" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+      <c r="A14" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="2"/>
+      <c r="B14" s="4" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" s="2"/>
+      <c r="B15" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16" s="2"/>
+      <c r="B16" s="4" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+      <c r="A17" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C17" s="2"/>
+      <c r="B17" s="3" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+      <c r="A18" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C18" s="2"/>
+      <c r="B18" s="3" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
+      <c r="A19" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C19" s="2"/>
+      <c r="B19" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="2"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="2"/>
+      <c r="B20" s="3"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="8" t="s">
+      <c r="B21" s="3"/>
+      <c r="C21" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
+      <c r="A22" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="4">
+      <c r="B22" s="3">
         <v>276</v>
       </c>
       <c r="C22" s="1" t="s">
@@ -1011,10 +955,10 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
+      <c r="A23" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="4">
+      <c r="B23" s="3">
         <v>277</v>
       </c>
       <c r="C23" s="1" t="s">
@@ -1022,10 +966,10 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
+      <c r="A24" t="s">
         <v>7</v>
       </c>
-      <c r="B24" s="4">
+      <c r="B24" s="3">
         <v>278</v>
       </c>
       <c r="C24" s="1" t="s">
@@ -1033,10 +977,10 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="7" t="s">
+      <c r="A25" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="4">
+      <c r="B25" s="3">
         <v>279</v>
       </c>
       <c r="C25" s="1" t="s">
@@ -1044,10 +988,10 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="7" t="s">
+      <c r="A26" t="s">
         <v>7</v>
       </c>
-      <c r="B26" s="4">
+      <c r="B26" s="3">
         <v>280</v>
       </c>
       <c r="C26" s="1" t="s">
@@ -1055,10 +999,10 @@
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="7" t="s">
+      <c r="A27" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="4">
+      <c r="B27" s="3">
         <v>281</v>
       </c>
       <c r="C27" s="1" t="s">
@@ -1066,10 +1010,10 @@
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
+      <c r="A28" t="s">
         <v>7</v>
       </c>
-      <c r="B28" s="4">
+      <c r="B28" s="3">
         <v>303</v>
       </c>
       <c r="C28" s="1" t="s">
@@ -1077,10 +1021,10 @@
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="7" t="s">
+      <c r="A29" t="s">
         <v>7</v>
       </c>
-      <c r="B29" s="4">
+      <c r="B29" s="3">
         <v>304</v>
       </c>
       <c r="C29" s="1" t="s">
@@ -1088,10 +1032,10 @@
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
+      <c r="A30" t="s">
         <v>7</v>
       </c>
-      <c r="B30" s="4">
+      <c r="B30" s="3">
         <v>305</v>
       </c>
       <c r="C30" s="1" t="s">
@@ -1099,10 +1043,10 @@
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="7" t="s">
+      <c r="A31" t="s">
         <v>7</v>
       </c>
-      <c r="B31" s="4">
+      <c r="B31" s="3">
         <v>320</v>
       </c>
       <c r="C31" s="1" t="s">
@@ -1110,10 +1054,10 @@
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="7" t="s">
+      <c r="A32" t="s">
         <v>7</v>
       </c>
-      <c r="B32" s="4">
+      <c r="B32" s="3">
         <v>321</v>
       </c>
       <c r="C32" s="1" t="s">
@@ -1121,10 +1065,10 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="7" t="s">
+      <c r="A33" t="s">
         <v>7</v>
       </c>
-      <c r="B33" s="4">
+      <c r="B33" s="3">
         <v>322</v>
       </c>
       <c r="C33" s="1" t="s">
@@ -1132,10 +1076,10 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="7" t="s">
+      <c r="A34" t="s">
         <v>7</v>
       </c>
-      <c r="B34" s="4">
+      <c r="B34" s="3">
         <v>323</v>
       </c>
       <c r="C34" s="1" t="s">
@@ -1143,10 +1087,10 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="7" t="s">
+      <c r="A35" t="s">
         <v>7</v>
       </c>
-      <c r="B35" s="4">
+      <c r="B35" s="3">
         <v>325</v>
       </c>
       <c r="C35" s="1" t="s">
@@ -1154,10 +1098,10 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="2" t="s">
+      <c r="A36" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="4">
+      <c r="B36" s="3">
         <v>331</v>
       </c>
       <c r="C36" s="1" t="s">
@@ -1168,7 +1112,7 @@
       <c r="A37" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B37" s="4">
+      <c r="B37" s="3">
         <v>330</v>
       </c>
       <c r="C37" s="1" t="s">
@@ -1176,10 +1120,10 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
+      <c r="A38" t="s">
         <v>7</v>
       </c>
-      <c r="B38" s="4">
+      <c r="B38" s="3">
         <v>341</v>
       </c>
       <c r="C38" s="1" t="s">
@@ -1190,7 +1134,7 @@
       <c r="A39" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B39" s="4">
+      <c r="B39" s="3">
         <v>340</v>
       </c>
       <c r="C39" s="1" t="s">
@@ -1198,10 +1142,10 @@
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="7" t="s">
+      <c r="A40" t="s">
         <v>26</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B40" s="4" t="s">
         <v>27</v>
       </c>
       <c r="C40" s="1" t="s">
@@ -1209,10 +1153,10 @@
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="7" t="s">
+      <c r="A41" t="s">
         <v>26</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="B41" s="4" t="s">
         <v>28</v>
       </c>
       <c r="C41" s="1" t="s">
@@ -1220,18 +1164,15 @@
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="7"/>
-      <c r="B42" s="4"/>
+      <c r="B42" s="3"/>
       <c r="C42" s="1"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="7"/>
-      <c r="B43" s="4"/>
+      <c r="B43" s="3"/>
       <c r="C43" s="1"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="7"/>
-      <c r="B44" s="4"/>
+      <c r="B44" s="3"/>
       <c r="C44" s="1"/>
     </row>
   </sheetData>
@@ -1249,8 +1190,8 @@
   <sheetPr codeName="List3"/>
   <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1261,293 +1202,255 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="10"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="10"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="10"/>
+      <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B6" s="3"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="A8" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="2"/>
+      <c r="B8" s="4"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="2"/>
+      <c r="B9" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="10"/>
+      <c r="B10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="5"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="2">
         <v>1440</v>
       </c>
-      <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="2">
         <v>5</v>
       </c>
-      <c r="C12" s="2"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" s="2"/>
+      <c r="B13" s="4" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+      <c r="A14" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="2"/>
+      <c r="B14" s="4" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" s="2"/>
+      <c r="B15" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16" s="2"/>
+      <c r="B16" s="4" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+      <c r="A17" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C17" s="2"/>
+      <c r="B17" s="3" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+      <c r="A18" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C18" s="2"/>
+      <c r="B18" s="3" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
+      <c r="A19" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="2"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="2"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="2"/>
+      <c r="B20" s="3"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="10" t="s">
+      <c r="B21" s="3"/>
+      <c r="C21" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A22" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B22" s="4"/>
+    <row r="22" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A22" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="3"/>
       <c r="C22" s="1"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="2"/>
-      <c r="B23" s="4"/>
+      <c r="B23" s="3"/>
       <c r="C23" s="1"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="2"/>
-      <c r="B24" s="4"/>
+      <c r="B24" s="3"/>
       <c r="C24" s="1"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="7"/>
-      <c r="B25" s="4"/>
+      <c r="B25" s="3"/>
       <c r="C25" s="1"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="7"/>
-      <c r="B26" s="4"/>
+      <c r="B26" s="3"/>
       <c r="C26" s="1"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="7"/>
-      <c r="B27" s="4"/>
+      <c r="B27" s="3"/>
       <c r="C27" s="1"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="2"/>
-      <c r="B28" s="4"/>
+      <c r="B28" s="3"/>
       <c r="C28" s="1"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="7"/>
-      <c r="B29" s="4"/>
+      <c r="B29" s="3"/>
       <c r="C29" s="1"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="2"/>
-      <c r="B30" s="4"/>
+      <c r="B30" s="3"/>
       <c r="C30" s="1"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="7"/>
-      <c r="B31" s="4"/>
+      <c r="B31" s="3"/>
       <c r="C31" s="1"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="7"/>
-      <c r="B32" s="4"/>
+      <c r="B32" s="3"/>
       <c r="C32" s="1"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="7"/>
-      <c r="B33" s="4"/>
+      <c r="B33" s="3"/>
       <c r="C33" s="1"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="7"/>
-      <c r="B34" s="4"/>
+      <c r="B34" s="3"/>
       <c r="C34" s="1"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="7"/>
-      <c r="B35" s="4"/>
+      <c r="B35" s="3"/>
       <c r="C35" s="1"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="2"/>
-      <c r="B36" s="4"/>
+      <c r="B36" s="3"/>
       <c r="C36" s="1"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="1"/>
-      <c r="B37" s="4"/>
+      <c r="B37" s="3"/>
       <c r="C37" s="1"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="2"/>
-      <c r="B38" s="4"/>
+      <c r="B38" s="3"/>
       <c r="C38" s="1"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
-      <c r="B39" s="4"/>
+      <c r="B39" s="3"/>
       <c r="C39" s="1"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="7"/>
-      <c r="B40" s="5"/>
+      <c r="B40" s="4"/>
       <c r="C40" s="1"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="7"/>
-      <c r="B41" s="5"/>
+      <c r="B41" s="4"/>
       <c r="C41" s="1"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="7"/>
-      <c r="B42" s="4"/>
+      <c r="B42" s="3"/>
       <c r="C42" s="1"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="7"/>
-      <c r="B43" s="4"/>
+      <c r="B43" s="3"/>
       <c r="C43" s="1"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="7"/>
-      <c r="B44" s="4"/>
+      <c r="B44" s="3"/>
       <c r="C44" s="1"/>
     </row>
   </sheetData>
@@ -1565,7 +1468,7 @@
   <sheetPr codeName="List4"/>
   <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -1577,301 +1480,264 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="10"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="10"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="10"/>
+      <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B6" s="3"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="A8" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="2"/>
+      <c r="B8" s="4"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="2"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="10"/>
+      <c r="C10" s="5"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="2"/>
+      <c r="B11" s="2"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="2">
         <v>5</v>
       </c>
-      <c r="C12" s="2"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" s="2"/>
+      <c r="B13" s="4" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+      <c r="A14" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="2"/>
+      <c r="B14" s="4" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" s="2"/>
+      <c r="B15" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16" s="2"/>
+      <c r="B16" s="4" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+      <c r="A17" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C17" s="2"/>
+      <c r="B17" s="3" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+      <c r="A18" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C18" s="2"/>
+      <c r="B18" s="3" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
+      <c r="A19" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="2"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="2"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="2"/>
+      <c r="B20" s="3"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="10" t="s">
+      <c r="B21" s="3"/>
+      <c r="C21" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>39</v>
-      </c>
       <c r="C23" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="2"/>
-      <c r="B24" s="4"/>
+      <c r="B24" s="3"/>
       <c r="C24" s="1"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="7"/>
-      <c r="B25" s="4"/>
+      <c r="B25" s="3"/>
       <c r="C25" s="1"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="7"/>
-      <c r="B26" s="4"/>
+      <c r="B26" s="3"/>
       <c r="C26" s="1"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="7"/>
-      <c r="B27" s="4"/>
+      <c r="B27" s="3"/>
       <c r="C27" s="1"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="2"/>
-      <c r="B28" s="4"/>
+      <c r="B28" s="3"/>
       <c r="C28" s="1"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="7"/>
-      <c r="B29" s="4"/>
+      <c r="B29" s="3"/>
       <c r="C29" s="1"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="2"/>
-      <c r="B30" s="4"/>
+      <c r="B30" s="3"/>
       <c r="C30" s="1"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="7"/>
-      <c r="B31" s="4"/>
+      <c r="B31" s="3"/>
       <c r="C31" s="1"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="7"/>
-      <c r="B32" s="4"/>
+      <c r="B32" s="3"/>
       <c r="C32" s="1"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="7"/>
-      <c r="B33" s="4"/>
+      <c r="B33" s="3"/>
       <c r="C33" s="1"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="7"/>
-      <c r="B34" s="4"/>
+      <c r="B34" s="3"/>
       <c r="C34" s="1"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="7"/>
-      <c r="B35" s="4"/>
+      <c r="B35" s="3"/>
       <c r="C35" s="1"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="2"/>
-      <c r="B36" s="4"/>
+      <c r="B36" s="3"/>
       <c r="C36" s="1"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="1"/>
-      <c r="B37" s="4"/>
+      <c r="B37" s="3"/>
       <c r="C37" s="1"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="2"/>
-      <c r="B38" s="4"/>
+      <c r="B38" s="3"/>
       <c r="C38" s="1"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
-      <c r="B39" s="4"/>
+      <c r="B39" s="3"/>
       <c r="C39" s="1"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="7"/>
-      <c r="B40" s="5"/>
+      <c r="B40" s="4"/>
       <c r="C40" s="1"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="7"/>
-      <c r="B41" s="5"/>
+      <c r="B41" s="4"/>
       <c r="C41" s="1"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="7"/>
-      <c r="B42" s="4"/>
+      <c r="B42" s="3"/>
       <c r="C42" s="1"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="7"/>
-      <c r="B43" s="4"/>
+      <c r="B43" s="3"/>
       <c r="C43" s="1"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="7"/>
-      <c r="B44" s="4"/>
+      <c r="B44" s="3"/>
       <c r="C44" s="1"/>
     </row>
   </sheetData>

</xml_diff>